<commit_message>
auto: displaying data in the Appoitment Follow-up form from the the appointment schedule form
</commit_message>
<xml_diff>
--- a/config/forms/app/viral.xlsx
+++ b/config/forms/app/viral.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="71">
   <si>
     <t>type</t>
   </si>
@@ -42,7 +42,7 @@
     <t>inputs</t>
   </si>
   <si>
-    <t>Appointment Follow-up</t>
+    <t>NO_LABEL</t>
   </si>
   <si>
     <t>./source = 'user'</t>
@@ -57,12 +57,18 @@
     <t>source</t>
   </si>
   <si>
-    <t>NO_LABEL</t>
-  </si>
-  <si>
     <t>source_id</t>
   </si>
   <si>
+    <t>my_field_viral</t>
+  </si>
+  <si>
+    <t>viral_field_notes</t>
+  </si>
+  <si>
+    <t>viral_field_date</t>
+  </si>
+  <si>
     <t>contact</t>
   </si>
   <si>
@@ -120,28 +126,28 @@
     <t>appoint</t>
   </si>
   <si>
-    <t>select_one type</t>
+    <t>note</t>
   </si>
   <si>
     <t>type1</t>
   </si>
   <si>
-    <t>Appointment Type</t>
+    <t xml:space="preserve">Appointment Type : ${my_field_viral} appointment </t>
   </si>
   <si>
     <t>due</t>
   </si>
   <si>
-    <t>Any notes about this Appointment?</t>
+    <t>Any notes about this Appointment?: ${viral_field_notes}</t>
+  </si>
+  <si>
+    <t>date1</t>
+  </si>
+  <si>
+    <t>Date of Appointment: ${viral_field_date}</t>
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>date1</t>
-  </si>
-  <si>
-    <t>Date of Appointment:</t>
   </si>
   <si>
     <t>date2</t>
@@ -181,25 +187,6 @@
     <t>Snooze task for 2 days</t>
   </si>
   <si>
-    <t>clinical</t>
-  </si>
-  <si>
-    <t>Clinical Appointment</t>
-  </si>
-  <si>
-    <t>social</t>
-  </si>
-  <si>
-    <t>Social Worker Appointment</t>
-  </si>
-  <si>
-    <t>case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case Manager Appointment
-</t>
-  </si>
-  <si>
     <t>Noted, I will follow-up with patient or care team as needed</t>
   </si>
   <si>
@@ -228,6 +215,9 @@
   </si>
   <si>
     <t>default_language</t>
+  </si>
+  <si>
+    <t>Appointment Follow-up</t>
   </si>
   <si>
     <t>pages</t>
@@ -326,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -344,6 +334,12 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -600,6 +596,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="18.38"/>
+    <col customWidth="1" min="2" max="2" width="20.88"/>
     <col customWidth="1" min="3" max="3" width="46.25"/>
     <col customWidth="1" min="6" max="6" width="20.0"/>
   </cols>
@@ -654,7 +651,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
@@ -668,10 +665,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
@@ -682,13 +679,13 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -696,82 +693,76 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1</v>
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
@@ -781,44 +772,48 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>25</v>
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>16</v>
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
@@ -828,58 +823,72 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>1</v>
+      <c r="A14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>27</v>
+      <c r="A18" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -889,116 +898,152 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="A20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="7" t="s">
-        <v>33</v>
-      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
+      <c r="B24" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="9" t="s">
+    <row r="25">
+      <c r="A25" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="9" t="s">
+      <c r="B25" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C25" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="9" t="s">
+    <row r="26">
+      <c r="A26" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="C26" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="9" t="s">
+    </row>
+    <row r="27">
+      <c r="A27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="9" t="s">
+      <c r="C27" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="9" t="s">
+    </row>
+    <row r="28">
+      <c r="A28" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="B28" s="11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="9" t="s">
+      <c r="C28" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="F28" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="G28" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="10" t="s">
-        <v>27</v>
+      <c r="B29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1021,7 +1066,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1031,80 +1076,47 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>52</v>
       </c>
+      <c r="B2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>56</v>
+      <c r="C4" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="C5" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1127,47 +1139,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="G1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="11" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="B2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="16" t="str">
+        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
+        <v>2022-07-25_15-09</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="E2" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="14" t="str">
-        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-13_19-08</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>